<commit_message>
Funcional coleta de informações individuais de cotas mês a mês
</commit_message>
<xml_diff>
--- a/cvm_to_learn/BD_CADASTRO_NUMERADO_AGO_TESTE.xlsx
+++ b/cvm_to_learn/BD_CADASTRO_NUMERADO_AGO_TESTE.xlsx
@@ -15,24 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>01.608.573/0001-65</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>04.288.966/0001-27</t>
-  </si>
-  <si>
-    <t>13.077.415/0001-05</t>
-  </si>
-  <si>
-    <t>13.077.418/0001-49</t>
-  </si>
-  <si>
-    <t>04.857.834/0001-79</t>
+    <t>58.877.827/0001-68</t>
   </si>
 </sst>
 </file>
@@ -40,7 +28,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,12 +39,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -88,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -96,19 +78,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -419,8 +392,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -428,32 +401,20 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
@@ -523,43 +484,43 @@
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
@@ -2096,1471 +2057,1471 @@
       <c r="B414" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="415" customHeight="1" ht="15.75">
-      <c r="A415" s="6"/>
+      <c r="A415" s="1"/>
       <c r="B415" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="416" customHeight="1" ht="15.75">
-      <c r="A416" s="6"/>
+      <c r="A416" s="1"/>
       <c r="B416" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="417" customHeight="1" ht="15.75">
-      <c r="A417" s="6"/>
+      <c r="A417" s="1"/>
       <c r="B417" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="418" customHeight="1" ht="15.75">
-      <c r="A418" s="6"/>
+      <c r="A418" s="1"/>
       <c r="B418" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="419" customHeight="1" ht="15.75">
-      <c r="A419" s="6"/>
+      <c r="A419" s="1"/>
       <c r="B419" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="420" customHeight="1" ht="15.75">
-      <c r="A420" s="6"/>
+      <c r="A420" s="1"/>
       <c r="B420" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="421" customHeight="1" ht="15.75">
-      <c r="A421" s="6"/>
+      <c r="A421" s="1"/>
       <c r="B421" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="422" customHeight="1" ht="15.75">
-      <c r="A422" s="6"/>
+      <c r="A422" s="1"/>
       <c r="B422" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="423" customHeight="1" ht="15.75">
-      <c r="A423" s="6"/>
+      <c r="A423" s="1"/>
       <c r="B423" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="424" customHeight="1" ht="15.75">
-      <c r="A424" s="6"/>
+      <c r="A424" s="1"/>
       <c r="B424" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="425" customHeight="1" ht="15.75">
-      <c r="A425" s="6"/>
+      <c r="A425" s="1"/>
       <c r="B425" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="426" customHeight="1" ht="15.75">
-      <c r="A426" s="6"/>
+      <c r="A426" s="1"/>
       <c r="B426" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="427" customHeight="1" ht="15.75">
-      <c r="A427" s="6"/>
+      <c r="A427" s="1"/>
       <c r="B427" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="428" customHeight="1" ht="15.75">
-      <c r="A428" s="6"/>
+      <c r="A428" s="1"/>
       <c r="B428" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="429" customHeight="1" ht="15.75">
-      <c r="A429" s="6"/>
+      <c r="A429" s="1"/>
       <c r="B429" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="430" customHeight="1" ht="15.75">
-      <c r="A430" s="6"/>
+      <c r="A430" s="1"/>
       <c r="B430" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="431" customHeight="1" ht="15.75">
-      <c r="A431" s="6"/>
+      <c r="A431" s="1"/>
       <c r="B431" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="432" customHeight="1" ht="15.75">
-      <c r="A432" s="6"/>
+      <c r="A432" s="1"/>
       <c r="B432" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="433" customHeight="1" ht="15.75">
-      <c r="A433" s="6"/>
+      <c r="A433" s="1"/>
       <c r="B433" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="434" customHeight="1" ht="15.75">
-      <c r="A434" s="6"/>
+      <c r="A434" s="1"/>
       <c r="B434" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="435" customHeight="1" ht="15.75">
-      <c r="A435" s="6"/>
+      <c r="A435" s="1"/>
       <c r="B435" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="436" customHeight="1" ht="15.75">
-      <c r="A436" s="6"/>
+      <c r="A436" s="1"/>
       <c r="B436" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="437" customHeight="1" ht="15.75">
-      <c r="A437" s="6"/>
+      <c r="A437" s="1"/>
       <c r="B437" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="438" customHeight="1" ht="15.75">
-      <c r="A438" s="6"/>
+      <c r="A438" s="1"/>
       <c r="B438" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="439" customHeight="1" ht="15.75">
-      <c r="A439" s="6"/>
+      <c r="A439" s="1"/>
       <c r="B439" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="440" customHeight="1" ht="15.75">
-      <c r="A440" s="6"/>
+      <c r="A440" s="1"/>
       <c r="B440" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="15.75">
-      <c r="A441" s="6"/>
+      <c r="A441" s="1"/>
       <c r="B441" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="442" customHeight="1" ht="15.75">
-      <c r="A442" s="6"/>
+      <c r="A442" s="1"/>
       <c r="B442" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="443" customHeight="1" ht="15.75">
-      <c r="A443" s="6"/>
+      <c r="A443" s="1"/>
       <c r="B443" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="444" customHeight="1" ht="15.75">
-      <c r="A444" s="6"/>
+      <c r="A444" s="1"/>
       <c r="B444" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="445" customHeight="1" ht="15.75">
-      <c r="A445" s="6"/>
+      <c r="A445" s="1"/>
       <c r="B445" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="446" customHeight="1" ht="15.75">
-      <c r="A446" s="6"/>
+      <c r="A446" s="1"/>
       <c r="B446" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="447" customHeight="1" ht="15.75">
-      <c r="A447" s="6"/>
+      <c r="A447" s="1"/>
       <c r="B447" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="448" customHeight="1" ht="15.75">
-      <c r="A448" s="6"/>
+      <c r="A448" s="1"/>
       <c r="B448" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="449" customHeight="1" ht="15.75">
-      <c r="A449" s="6"/>
+      <c r="A449" s="1"/>
       <c r="B449" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="450" customHeight="1" ht="15.75">
-      <c r="A450" s="6"/>
+      <c r="A450" s="1"/>
       <c r="B450" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="451" customHeight="1" ht="15.75">
-      <c r="A451" s="6"/>
+      <c r="A451" s="1"/>
       <c r="B451" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="452" customHeight="1" ht="15.75">
-      <c r="A452" s="6"/>
+      <c r="A452" s="1"/>
       <c r="B452" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="15.75">
-      <c r="A453" s="6"/>
+      <c r="A453" s="1"/>
       <c r="B453" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="454" customHeight="1" ht="15.75">
-      <c r="A454" s="6"/>
+      <c r="A454" s="1"/>
       <c r="B454" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="455" customHeight="1" ht="15.75">
-      <c r="A455" s="6"/>
+      <c r="A455" s="1"/>
       <c r="B455" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="456" customHeight="1" ht="15.75">
-      <c r="A456" s="6"/>
+      <c r="A456" s="1"/>
       <c r="B456" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="457" customHeight="1" ht="15.75">
-      <c r="A457" s="6"/>
+      <c r="A457" s="1"/>
       <c r="B457" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="458" customHeight="1" ht="15.75">
-      <c r="A458" s="6"/>
+      <c r="A458" s="1"/>
       <c r="B458" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="459" customHeight="1" ht="15.75">
-      <c r="A459" s="6"/>
+      <c r="A459" s="1"/>
       <c r="B459" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="460" customHeight="1" ht="15.75">
-      <c r="A460" s="6"/>
+      <c r="A460" s="1"/>
       <c r="B460" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="461" customHeight="1" ht="15.75">
-      <c r="A461" s="6"/>
+      <c r="A461" s="1"/>
       <c r="B461" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="462" customHeight="1" ht="15.75">
-      <c r="A462" s="6"/>
+      <c r="A462" s="1"/>
       <c r="B462" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="463" customHeight="1" ht="15.75">
-      <c r="A463" s="6"/>
+      <c r="A463" s="1"/>
       <c r="B463" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="464" customHeight="1" ht="15.75">
-      <c r="A464" s="6"/>
+      <c r="A464" s="1"/>
       <c r="B464" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="465" customHeight="1" ht="15.75">
-      <c r="A465" s="6"/>
+      <c r="A465" s="1"/>
       <c r="B465" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="466" customHeight="1" ht="15.75">
-      <c r="A466" s="6"/>
+      <c r="A466" s="1"/>
       <c r="B466" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="467" customHeight="1" ht="15.75">
-      <c r="A467" s="6"/>
+      <c r="A467" s="1"/>
       <c r="B467" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="468" customHeight="1" ht="15.75">
-      <c r="A468" s="6"/>
+      <c r="A468" s="1"/>
       <c r="B468" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="469" customHeight="1" ht="15.75">
-      <c r="A469" s="6"/>
+      <c r="A469" s="1"/>
       <c r="B469" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="470" customHeight="1" ht="15.75">
-      <c r="A470" s="6"/>
+      <c r="A470" s="1"/>
       <c r="B470" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="471" customHeight="1" ht="15.75">
-      <c r="A471" s="6"/>
+      <c r="A471" s="1"/>
       <c r="B471" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="472" customHeight="1" ht="15.75">
-      <c r="A472" s="6"/>
+      <c r="A472" s="1"/>
       <c r="B472" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="473" customHeight="1" ht="15.75">
-      <c r="A473" s="6"/>
+      <c r="A473" s="1"/>
       <c r="B473" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="474" customHeight="1" ht="15.75">
-      <c r="A474" s="6"/>
+      <c r="A474" s="1"/>
       <c r="B474" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="475" customHeight="1" ht="15.75">
-      <c r="A475" s="6"/>
+      <c r="A475" s="1"/>
       <c r="B475" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="476" customHeight="1" ht="15.75">
-      <c r="A476" s="6"/>
+      <c r="A476" s="1"/>
       <c r="B476" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="477" customHeight="1" ht="15.75">
-      <c r="A477" s="6"/>
+      <c r="A477" s="1"/>
       <c r="B477" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="478" customHeight="1" ht="15.75">
-      <c r="A478" s="6"/>
+      <c r="A478" s="1"/>
       <c r="B478" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="479" customHeight="1" ht="15.75">
-      <c r="A479" s="6"/>
+      <c r="A479" s="1"/>
       <c r="B479" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="480" customHeight="1" ht="15.75">
-      <c r="A480" s="6"/>
+      <c r="A480" s="1"/>
       <c r="B480" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="481" customHeight="1" ht="15.75">
-      <c r="A481" s="6"/>
+      <c r="A481" s="1"/>
       <c r="B481" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="482" customHeight="1" ht="15.75">
-      <c r="A482" s="6"/>
+      <c r="A482" s="1"/>
       <c r="B482" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="483" customHeight="1" ht="15.75">
-      <c r="A483" s="6"/>
+      <c r="A483" s="1"/>
       <c r="B483" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="484" customHeight="1" ht="15.75">
-      <c r="A484" s="6"/>
+      <c r="A484" s="1"/>
       <c r="B484" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="485" customHeight="1" ht="15.75">
-      <c r="A485" s="6"/>
+      <c r="A485" s="1"/>
       <c r="B485" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="486" customHeight="1" ht="15.75">
-      <c r="A486" s="6"/>
+      <c r="A486" s="1"/>
       <c r="B486" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="487" customHeight="1" ht="15.75">
-      <c r="A487" s="6"/>
+      <c r="A487" s="1"/>
       <c r="B487" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="488" customHeight="1" ht="15.75">
-      <c r="A488" s="6"/>
+      <c r="A488" s="1"/>
       <c r="B488" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="489" customHeight="1" ht="15.75">
-      <c r="A489" s="6"/>
+      <c r="A489" s="1"/>
       <c r="B489" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="490" customHeight="1" ht="15.75">
-      <c r="A490" s="6"/>
+      <c r="A490" s="1"/>
       <c r="B490" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="491" customHeight="1" ht="15.75">
-      <c r="A491" s="6"/>
+      <c r="A491" s="1"/>
       <c r="B491" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="492" customHeight="1" ht="15.75">
-      <c r="A492" s="6"/>
+      <c r="A492" s="1"/>
       <c r="B492" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="493" customHeight="1" ht="15.75">
-      <c r="A493" s="6"/>
+      <c r="A493" s="1"/>
       <c r="B493" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="494" customHeight="1" ht="15.75">
-      <c r="A494" s="6"/>
+      <c r="A494" s="1"/>
       <c r="B494" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="495" customHeight="1" ht="15.75">
-      <c r="A495" s="6"/>
+      <c r="A495" s="1"/>
       <c r="B495" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="496" customHeight="1" ht="15.75">
-      <c r="A496" s="6"/>
+      <c r="A496" s="1"/>
       <c r="B496" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="497" customHeight="1" ht="15.75">
-      <c r="A497" s="6"/>
+      <c r="A497" s="1"/>
       <c r="B497" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="498" customHeight="1" ht="15.75">
-      <c r="A498" s="6"/>
+      <c r="A498" s="1"/>
       <c r="B498" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="499" customHeight="1" ht="15.75">
-      <c r="A499" s="6"/>
+      <c r="A499" s="1"/>
       <c r="B499" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="500" customHeight="1" ht="15.75">
-      <c r="A500" s="6"/>
+      <c r="A500" s="1"/>
       <c r="B500" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="501" customHeight="1" ht="15.75">
-      <c r="A501" s="6"/>
+      <c r="A501" s="1"/>
       <c r="B501" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="502" customHeight="1" ht="15.75">
-      <c r="A502" s="6"/>
+      <c r="A502" s="1"/>
       <c r="B502" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="503" customHeight="1" ht="15.75">
-      <c r="A503" s="6"/>
+      <c r="A503" s="1"/>
       <c r="B503" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="504" customHeight="1" ht="15.75">
-      <c r="A504" s="6"/>
+      <c r="A504" s="1"/>
       <c r="B504" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="505" customHeight="1" ht="15.75">
-      <c r="A505" s="6"/>
+      <c r="A505" s="1"/>
       <c r="B505" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="506" customHeight="1" ht="15.75">
-      <c r="A506" s="6"/>
+      <c r="A506" s="1"/>
       <c r="B506" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="507" customHeight="1" ht="15.75">
-      <c r="A507" s="6"/>
+      <c r="A507" s="1"/>
       <c r="B507" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="508" customHeight="1" ht="15.75">
-      <c r="A508" s="6"/>
+      <c r="A508" s="1"/>
       <c r="B508" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="509" customHeight="1" ht="15.75">
-      <c r="A509" s="6"/>
+      <c r="A509" s="1"/>
       <c r="B509" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="510" customHeight="1" ht="15.75">
-      <c r="A510" s="6"/>
+      <c r="A510" s="1"/>
       <c r="B510" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="511" customHeight="1" ht="15.75">
-      <c r="A511" s="6"/>
+      <c r="A511" s="1"/>
       <c r="B511" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="512" customHeight="1" ht="15.75">
-      <c r="A512" s="6"/>
+      <c r="A512" s="1"/>
       <c r="B512" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="513" customHeight="1" ht="15.75">
-      <c r="A513" s="6"/>
+      <c r="A513" s="1"/>
       <c r="B513" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="514" customHeight="1" ht="15.75">
-      <c r="A514" s="6"/>
+      <c r="A514" s="1"/>
       <c r="B514" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="515" customHeight="1" ht="15.75">
-      <c r="A515" s="6"/>
+      <c r="A515" s="1"/>
       <c r="B515" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="516" customHeight="1" ht="15.75">
-      <c r="A516" s="6"/>
+      <c r="A516" s="1"/>
       <c r="B516" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="517" customHeight="1" ht="15.75">
-      <c r="A517" s="6"/>
+      <c r="A517" s="1"/>
       <c r="B517" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="518" customHeight="1" ht="15.75">
-      <c r="A518" s="6"/>
+      <c r="A518" s="1"/>
       <c r="B518" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="519" customHeight="1" ht="15.75">
-      <c r="A519" s="6"/>
+      <c r="A519" s="1"/>
       <c r="B519" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="520" customHeight="1" ht="15.75">
-      <c r="A520" s="6"/>
+      <c r="A520" s="1"/>
       <c r="B520" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="521" customHeight="1" ht="15.75">
-      <c r="A521" s="6"/>
+      <c r="A521" s="1"/>
       <c r="B521" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="522" customHeight="1" ht="15.75">
-      <c r="A522" s="6"/>
+      <c r="A522" s="1"/>
       <c r="B522" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="523" customHeight="1" ht="15.75">
-      <c r="A523" s="6"/>
+      <c r="A523" s="1"/>
       <c r="B523" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="524" customHeight="1" ht="15.75">
-      <c r="A524" s="6"/>
+      <c r="A524" s="1"/>
       <c r="B524" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="525" customHeight="1" ht="15.75">
-      <c r="A525" s="6"/>
+      <c r="A525" s="1"/>
       <c r="B525" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="526" customHeight="1" ht="15.75">
-      <c r="A526" s="6"/>
+      <c r="A526" s="1"/>
       <c r="B526" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="527" customHeight="1" ht="15.75">
-      <c r="A527" s="6"/>
+      <c r="A527" s="1"/>
       <c r="B527" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="528" customHeight="1" ht="15.75">
-      <c r="A528" s="6"/>
+      <c r="A528" s="1"/>
       <c r="B528" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="529" customHeight="1" ht="15.75">
-      <c r="A529" s="6"/>
+      <c r="A529" s="1"/>
       <c r="B529" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="530" customHeight="1" ht="15.75">
-      <c r="A530" s="6"/>
+      <c r="A530" s="1"/>
       <c r="B530" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="531" customHeight="1" ht="15.75">
-      <c r="A531" s="6"/>
+      <c r="A531" s="1"/>
       <c r="B531" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="532" customHeight="1" ht="15.75">
-      <c r="A532" s="6"/>
+      <c r="A532" s="1"/>
       <c r="B532" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="533" customHeight="1" ht="15.75">
-      <c r="A533" s="6"/>
+      <c r="A533" s="1"/>
       <c r="B533" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="534" customHeight="1" ht="15.75">
-      <c r="A534" s="6"/>
+      <c r="A534" s="1"/>
       <c r="B534" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="535" customHeight="1" ht="15.75">
-      <c r="A535" s="6"/>
+      <c r="A535" s="1"/>
       <c r="B535" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="536" customHeight="1" ht="15.75">
-      <c r="A536" s="6"/>
+      <c r="A536" s="1"/>
       <c r="B536" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="537" customHeight="1" ht="15.75">
-      <c r="A537" s="6"/>
+      <c r="A537" s="1"/>
       <c r="B537" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="538" customHeight="1" ht="15.75">
-      <c r="A538" s="6"/>
+      <c r="A538" s="1"/>
       <c r="B538" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="539" customHeight="1" ht="15.75">
-      <c r="A539" s="6"/>
+      <c r="A539" s="1"/>
       <c r="B539" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="540" customHeight="1" ht="15.75">
-      <c r="A540" s="6"/>
+      <c r="A540" s="1"/>
       <c r="B540" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="541" customHeight="1" ht="15.75">
-      <c r="A541" s="6"/>
+      <c r="A541" s="1"/>
       <c r="B541" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="542" customHeight="1" ht="15.75">
-      <c r="A542" s="6"/>
+      <c r="A542" s="1"/>
       <c r="B542" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="543" customHeight="1" ht="15.75">
-      <c r="A543" s="6"/>
+      <c r="A543" s="1"/>
       <c r="B543" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="544" customHeight="1" ht="15.75">
-      <c r="A544" s="6"/>
+      <c r="A544" s="1"/>
       <c r="B544" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="545" customHeight="1" ht="15.75">
-      <c r="A545" s="6"/>
+      <c r="A545" s="1"/>
       <c r="B545" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="546" customHeight="1" ht="15.75">
-      <c r="A546" s="6"/>
+      <c r="A546" s="1"/>
       <c r="B546" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="547" customHeight="1" ht="15.75">
-      <c r="A547" s="6"/>
+      <c r="A547" s="1"/>
       <c r="B547" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="548" customHeight="1" ht="15.75">
-      <c r="A548" s="6"/>
+      <c r="A548" s="1"/>
       <c r="B548" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="549" customHeight="1" ht="15.75">
-      <c r="A549" s="6"/>
+      <c r="A549" s="1"/>
       <c r="B549" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="550" customHeight="1" ht="15.75">
-      <c r="A550" s="6"/>
+      <c r="A550" s="1"/>
       <c r="B550" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="551" customHeight="1" ht="15.75">
-      <c r="A551" s="6"/>
+      <c r="A551" s="1"/>
       <c r="B551" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="552" customHeight="1" ht="15.75">
-      <c r="A552" s="6"/>
+      <c r="A552" s="1"/>
       <c r="B552" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="553" customHeight="1" ht="15.75">
-      <c r="A553" s="6"/>
+      <c r="A553" s="1"/>
       <c r="B553" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="554" customHeight="1" ht="15.75">
-      <c r="A554" s="6"/>
+      <c r="A554" s="1"/>
       <c r="B554" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="555" customHeight="1" ht="15.75">
-      <c r="A555" s="6"/>
+      <c r="A555" s="1"/>
       <c r="B555" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="556" customHeight="1" ht="15.75">
-      <c r="A556" s="6"/>
+      <c r="A556" s="1"/>
       <c r="B556" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="557" customHeight="1" ht="15.75">
-      <c r="A557" s="6"/>
+      <c r="A557" s="1"/>
       <c r="B557" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="558" customHeight="1" ht="15.75">
-      <c r="A558" s="6"/>
+      <c r="A558" s="1"/>
       <c r="B558" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="559" customHeight="1" ht="15.75">
-      <c r="A559" s="6"/>
+      <c r="A559" s="1"/>
       <c r="B559" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="560" customHeight="1" ht="15.75">
-      <c r="A560" s="6"/>
+      <c r="A560" s="1"/>
       <c r="B560" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="561" customHeight="1" ht="15.75">
-      <c r="A561" s="6"/>
+      <c r="A561" s="1"/>
       <c r="B561" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="562" customHeight="1" ht="15.75">
-      <c r="A562" s="6"/>
+      <c r="A562" s="1"/>
       <c r="B562" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="563" customHeight="1" ht="15.75">
-      <c r="A563" s="6"/>
+      <c r="A563" s="1"/>
       <c r="B563" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="564" customHeight="1" ht="15.75">
-      <c r="A564" s="6"/>
+      <c r="A564" s="1"/>
       <c r="B564" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="565" customHeight="1" ht="15.75">
-      <c r="A565" s="6"/>
+      <c r="A565" s="1"/>
       <c r="B565" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="566" customHeight="1" ht="15.75">
-      <c r="A566" s="6"/>
+      <c r="A566" s="1"/>
       <c r="B566" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="567" customHeight="1" ht="15.75">
-      <c r="A567" s="6"/>
+      <c r="A567" s="1"/>
       <c r="B567" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="568" customHeight="1" ht="15.75">
-      <c r="A568" s="6"/>
+      <c r="A568" s="1"/>
       <c r="B568" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="569" customHeight="1" ht="15.75">
-      <c r="A569" s="6"/>
+      <c r="A569" s="1"/>
       <c r="B569" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="570" customHeight="1" ht="15.75">
-      <c r="A570" s="6"/>
+      <c r="A570" s="1"/>
       <c r="B570" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="571" customHeight="1" ht="15.75">
-      <c r="A571" s="6"/>
+      <c r="A571" s="1"/>
       <c r="B571" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="572" customHeight="1" ht="15.75">
-      <c r="A572" s="6"/>
+      <c r="A572" s="1"/>
       <c r="B572" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="573" customHeight="1" ht="15.75">
-      <c r="A573" s="6"/>
+      <c r="A573" s="1"/>
       <c r="B573" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="574" customHeight="1" ht="15.75">
-      <c r="A574" s="6"/>
+      <c r="A574" s="1"/>
       <c r="B574" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="575" customHeight="1" ht="15.75">
-      <c r="A575" s="6"/>
+      <c r="A575" s="1"/>
       <c r="B575" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="576" customHeight="1" ht="15.75">
-      <c r="A576" s="6"/>
+      <c r="A576" s="1"/>
       <c r="B576" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="577" customHeight="1" ht="15.75">
-      <c r="A577" s="6"/>
+      <c r="A577" s="1"/>
       <c r="B577" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="578" customHeight="1" ht="15.75">
-      <c r="A578" s="6"/>
+      <c r="A578" s="1"/>
       <c r="B578" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="579" customHeight="1" ht="15.75">
-      <c r="A579" s="6"/>
+      <c r="A579" s="1"/>
       <c r="B579" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="580" customHeight="1" ht="15.75">
-      <c r="A580" s="6"/>
+      <c r="A580" s="1"/>
       <c r="B580" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="581" customHeight="1" ht="15.75">
-      <c r="A581" s="6"/>
+      <c r="A581" s="1"/>
       <c r="B581" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="582" customHeight="1" ht="15.75">
-      <c r="A582" s="6"/>
+      <c r="A582" s="1"/>
       <c r="B582" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="583" customHeight="1" ht="15.75">
-      <c r="A583" s="6"/>
+      <c r="A583" s="1"/>
       <c r="B583" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="584" customHeight="1" ht="15.75">
-      <c r="A584" s="6"/>
+      <c r="A584" s="1"/>
       <c r="B584" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="585" customHeight="1" ht="15.75">
-      <c r="A585" s="6"/>
+      <c r="A585" s="1"/>
       <c r="B585" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="586" customHeight="1" ht="15.75">
-      <c r="A586" s="6"/>
+      <c r="A586" s="1"/>
       <c r="B586" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="587" customHeight="1" ht="15.75">
-      <c r="A587" s="6"/>
+      <c r="A587" s="1"/>
       <c r="B587" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="588" customHeight="1" ht="15.75">
-      <c r="A588" s="6"/>
+      <c r="A588" s="1"/>
       <c r="B588" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="589" customHeight="1" ht="15.75">
-      <c r="A589" s="6"/>
+      <c r="A589" s="1"/>
       <c r="B589" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="590" customHeight="1" ht="15.75">
-      <c r="A590" s="6"/>
+      <c r="A590" s="1"/>
       <c r="B590" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="591" customHeight="1" ht="15.75">
-      <c r="A591" s="6"/>
+      <c r="A591" s="1"/>
       <c r="B591" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="592" customHeight="1" ht="15.75">
-      <c r="A592" s="6"/>
+      <c r="A592" s="1"/>
       <c r="B592" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="593" customHeight="1" ht="15.75">
-      <c r="A593" s="6"/>
+      <c r="A593" s="1"/>
       <c r="B593" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="594" customHeight="1" ht="15.75">
-      <c r="A594" s="6"/>
+      <c r="A594" s="1"/>
       <c r="B594" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="595" customHeight="1" ht="15.75">
-      <c r="A595" s="6"/>
+      <c r="A595" s="1"/>
       <c r="B595" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="596" customHeight="1" ht="15.75">
-      <c r="A596" s="6"/>
+      <c r="A596" s="1"/>
       <c r="B596" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="597" customHeight="1" ht="15.75">
-      <c r="A597" s="6"/>
+      <c r="A597" s="1"/>
       <c r="B597" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="598" customHeight="1" ht="15.75">
-      <c r="A598" s="6"/>
+      <c r="A598" s="1"/>
       <c r="B598" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="599" customHeight="1" ht="15.75">
-      <c r="A599" s="6"/>
+      <c r="A599" s="1"/>
       <c r="B599" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="600" customHeight="1" ht="15.75">
-      <c r="A600" s="6"/>
+      <c r="A600" s="1"/>
       <c r="B600" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="601" customHeight="1" ht="15.75">
-      <c r="A601" s="6"/>
+      <c r="A601" s="1"/>
       <c r="B601" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="602" customHeight="1" ht="15.75">
-      <c r="A602" s="6"/>
+      <c r="A602" s="1"/>
       <c r="B602" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="603" customHeight="1" ht="15.75">
-      <c r="A603" s="6"/>
+      <c r="A603" s="1"/>
       <c r="B603" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="604" customHeight="1" ht="15.75">
-      <c r="A604" s="6"/>
+      <c r="A604" s="1"/>
       <c r="B604" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="605" customHeight="1" ht="15.75">
-      <c r="A605" s="6"/>
+      <c r="A605" s="1"/>
       <c r="B605" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="606" customHeight="1" ht="15.75">
-      <c r="A606" s="6"/>
+      <c r="A606" s="1"/>
       <c r="B606" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="607" customHeight="1" ht="15.75">
-      <c r="A607" s="6"/>
+      <c r="A607" s="1"/>
       <c r="B607" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="608" customHeight="1" ht="15.75">
-      <c r="A608" s="6"/>
+      <c r="A608" s="1"/>
       <c r="B608" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="609" customHeight="1" ht="15.75">
-      <c r="A609" s="6"/>
+      <c r="A609" s="1"/>
       <c r="B609" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="610" customHeight="1" ht="15.75">
-      <c r="A610" s="6"/>
+      <c r="A610" s="1"/>
       <c r="B610" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="611" customHeight="1" ht="15.75">
-      <c r="A611" s="6"/>
+      <c r="A611" s="1"/>
       <c r="B611" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="612" customHeight="1" ht="15.75">
-      <c r="A612" s="6"/>
+      <c r="A612" s="1"/>
       <c r="B612" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="613" customHeight="1" ht="15.75">
-      <c r="A613" s="6"/>
+      <c r="A613" s="1"/>
       <c r="B613" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="614" customHeight="1" ht="15.75">
-      <c r="A614" s="6"/>
+      <c r="A614" s="1"/>
       <c r="B614" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="615" customHeight="1" ht="15.75">
-      <c r="A615" s="6"/>
+      <c r="A615" s="1"/>
       <c r="B615" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="616" customHeight="1" ht="15.75">
-      <c r="A616" s="6"/>
+      <c r="A616" s="1"/>
       <c r="B616" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="617" customHeight="1" ht="15.75">
-      <c r="A617" s="6"/>
+      <c r="A617" s="1"/>
       <c r="B617" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="618" customHeight="1" ht="15.75">
-      <c r="A618" s="6"/>
+      <c r="A618" s="1"/>
       <c r="B618" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="619" customHeight="1" ht="15.75">
-      <c r="A619" s="6"/>
+      <c r="A619" s="1"/>
       <c r="B619" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="620" customHeight="1" ht="15.75">
-      <c r="A620" s="6"/>
+      <c r="A620" s="1"/>
       <c r="B620" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="621" customHeight="1" ht="15.75">
-      <c r="A621" s="6"/>
+      <c r="A621" s="1"/>
       <c r="B621" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="622" customHeight="1" ht="15.75">
-      <c r="A622" s="6"/>
+      <c r="A622" s="1"/>
       <c r="B622" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="623" customHeight="1" ht="15.75">
-      <c r="A623" s="6"/>
+      <c r="A623" s="1"/>
       <c r="B623" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="624" customHeight="1" ht="15.75">
-      <c r="A624" s="6"/>
+      <c r="A624" s="1"/>
       <c r="B624" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="625" customHeight="1" ht="15.75">
-      <c r="A625" s="6"/>
+      <c r="A625" s="1"/>
       <c r="B625" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="626" customHeight="1" ht="15.75">
-      <c r="A626" s="6"/>
+      <c r="A626" s="1"/>
       <c r="B626" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="627" customHeight="1" ht="15.75">
-      <c r="A627" s="6"/>
+      <c r="A627" s="1"/>
       <c r="B627" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="628" customHeight="1" ht="15.75">
-      <c r="A628" s="6"/>
+      <c r="A628" s="1"/>
       <c r="B628" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="629" customHeight="1" ht="15.75">
-      <c r="A629" s="6"/>
+      <c r="A629" s="1"/>
       <c r="B629" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="630" customHeight="1" ht="15.75">
-      <c r="A630" s="6"/>
+      <c r="A630" s="1"/>
       <c r="B630" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="631" customHeight="1" ht="15.75">
-      <c r="A631" s="6"/>
+      <c r="A631" s="1"/>
       <c r="B631" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="632" customHeight="1" ht="15.75">
-      <c r="A632" s="6"/>
+      <c r="A632" s="1"/>
       <c r="B632" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="633" customHeight="1" ht="15.75">
-      <c r="A633" s="6"/>
+      <c r="A633" s="1"/>
       <c r="B633" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="634" customHeight="1" ht="15.75">
-      <c r="A634" s="6"/>
+      <c r="A634" s="1"/>
       <c r="B634" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="635" customHeight="1" ht="15.75">
-      <c r="A635" s="6"/>
+      <c r="A635" s="1"/>
       <c r="B635" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="636" customHeight="1" ht="15.75">
-      <c r="A636" s="6"/>
+      <c r="A636" s="1"/>
       <c r="B636" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="637" customHeight="1" ht="15.75">
-      <c r="A637" s="6"/>
+      <c r="A637" s="1"/>
       <c r="B637" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="638" customHeight="1" ht="15.75">
-      <c r="A638" s="6"/>
+      <c r="A638" s="1"/>
       <c r="B638" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="639" customHeight="1" ht="15.75">
-      <c r="A639" s="6"/>
+      <c r="A639" s="1"/>
       <c r="B639" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="640" customHeight="1" ht="15.75">
-      <c r="A640" s="6"/>
+      <c r="A640" s="1"/>
       <c r="B640" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="641" customHeight="1" ht="15.75">
-      <c r="A641" s="6"/>
+      <c r="A641" s="1"/>
       <c r="B641" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="642" customHeight="1" ht="15.75">
-      <c r="A642" s="6"/>
+      <c r="A642" s="1"/>
       <c r="B642" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="643" customHeight="1" ht="15.75">
-      <c r="A643" s="6"/>
+      <c r="A643" s="1"/>
       <c r="B643" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="644" customHeight="1" ht="15.75">
-      <c r="A644" s="6"/>
+      <c r="A644" s="1"/>
       <c r="B644" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="645" customHeight="1" ht="15.75">
-      <c r="A645" s="6"/>
+      <c r="A645" s="1"/>
       <c r="B645" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="646" customHeight="1" ht="15.75">
-      <c r="A646" s="6"/>
+      <c r="A646" s="1"/>
       <c r="B646" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="647" customHeight="1" ht="15.75">
-      <c r="A647" s="6"/>
+      <c r="A647" s="1"/>
       <c r="B647" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="648" customHeight="1" ht="15.75">
-      <c r="A648" s="6"/>
+      <c r="A648" s="1"/>
       <c r="B648" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="649" customHeight="1" ht="15.75">
-      <c r="A649" s="6"/>
+      <c r="A649" s="1"/>
       <c r="B649" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="650" customHeight="1" ht="15.75">
-      <c r="A650" s="6"/>
+      <c r="A650" s="1"/>
       <c r="B650" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="651" customHeight="1" ht="15.75">
-      <c r="A651" s="6"/>
+      <c r="A651" s="1"/>
       <c r="B651" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="652" customHeight="1" ht="15.75">
-      <c r="A652" s="6"/>
+      <c r="A652" s="1"/>
       <c r="B652" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="653" customHeight="1" ht="15.75">
-      <c r="A653" s="6"/>
+      <c r="A653" s="1"/>
       <c r="B653" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="654" customHeight="1" ht="15.75">
-      <c r="A654" s="6"/>
+      <c r="A654" s="1"/>
       <c r="B654" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="655" customHeight="1" ht="15.75">
-      <c r="A655" s="6"/>
+      <c r="A655" s="1"/>
       <c r="B655" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="656" customHeight="1" ht="15.75">
-      <c r="A656" s="6"/>
+      <c r="A656" s="1"/>
       <c r="B656" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="657" customHeight="1" ht="15.75">
-      <c r="A657" s="6"/>
+      <c r="A657" s="1"/>
       <c r="B657" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="658" customHeight="1" ht="15.75">
-      <c r="A658" s="6"/>
+      <c r="A658" s="1"/>
       <c r="B658" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="659" customHeight="1" ht="15.75">
-      <c r="A659" s="6"/>
+      <c r="A659" s="1"/>
       <c r="B659" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="660" customHeight="1" ht="15.75">
-      <c r="A660" s="6"/>
+      <c r="A660" s="1"/>
       <c r="B660" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="661" customHeight="1" ht="15.75">
-      <c r="A661" s="6"/>
+      <c r="A661" s="1"/>
       <c r="B661" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="662" customHeight="1" ht="15.75">
-      <c r="A662" s="6"/>
+      <c r="A662" s="1"/>
       <c r="B662" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="663" customHeight="1" ht="15.75">
-      <c r="A663" s="6"/>
+      <c r="A663" s="1"/>
       <c r="B663" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="664" customHeight="1" ht="15.75">
-      <c r="A664" s="6"/>
+      <c r="A664" s="1"/>
       <c r="B664" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="665" customHeight="1" ht="15.75">
-      <c r="A665" s="6"/>
+      <c r="A665" s="1"/>
       <c r="B665" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="666" customHeight="1" ht="15.75">
-      <c r="A666" s="6"/>
+      <c r="A666" s="1"/>
       <c r="B666" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="667" customHeight="1" ht="15.75">
-      <c r="A667" s="6"/>
+      <c r="A667" s="1"/>
       <c r="B667" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="668" customHeight="1" ht="15.75">
-      <c r="A668" s="6"/>
+      <c r="A668" s="1"/>
       <c r="B668" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="669" customHeight="1" ht="15.75">
-      <c r="A669" s="6"/>
+      <c r="A669" s="1"/>
       <c r="B669" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="670" customHeight="1" ht="15.75">
-      <c r="A670" s="6"/>
+      <c r="A670" s="1"/>
       <c r="B670" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="671" customHeight="1" ht="15.75">
-      <c r="A671" s="6"/>
+      <c r="A671" s="1"/>
       <c r="B671" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="672" customHeight="1" ht="15.75">
-      <c r="A672" s="6"/>
+      <c r="A672" s="1"/>
       <c r="B672" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="673" customHeight="1" ht="15.75">
-      <c r="A673" s="6"/>
+      <c r="A673" s="1"/>
       <c r="B673" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="674" customHeight="1" ht="15.75">
-      <c r="A674" s="6"/>
+      <c r="A674" s="1"/>
       <c r="B674" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="675" customHeight="1" ht="15.75">
-      <c r="A675" s="6"/>
+      <c r="A675" s="1"/>
       <c r="B675" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="676" customHeight="1" ht="15.75">
-      <c r="A676" s="6"/>
+      <c r="A676" s="1"/>
       <c r="B676" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="677" customHeight="1" ht="15.75">
-      <c r="A677" s="6"/>
+      <c r="A677" s="1"/>
       <c r="B677" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="678" customHeight="1" ht="15.75">
-      <c r="A678" s="6"/>
+      <c r="A678" s="1"/>
       <c r="B678" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="679" customHeight="1" ht="15.75">
-      <c r="A679" s="6"/>
+      <c r="A679" s="1"/>
       <c r="B679" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="680" customHeight="1" ht="15.75">
-      <c r="A680" s="6"/>
+      <c r="A680" s="1"/>
       <c r="B680" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="681" customHeight="1" ht="15.75">
-      <c r="A681" s="6"/>
+      <c r="A681" s="1"/>
       <c r="B681" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="682" customHeight="1" ht="15.75">
-      <c r="A682" s="6"/>
+      <c r="A682" s="1"/>
       <c r="B682" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="683" customHeight="1" ht="15.75">
-      <c r="A683" s="6"/>
+      <c r="A683" s="1"/>
       <c r="B683" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="684" customHeight="1" ht="15.75">
-      <c r="A684" s="6"/>
+      <c r="A684" s="1"/>
       <c r="B684" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="685" customHeight="1" ht="15.75">
-      <c r="A685" s="6"/>
+      <c r="A685" s="1"/>
       <c r="B685" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="686" customHeight="1" ht="15.75">
-      <c r="A686" s="6"/>
+      <c r="A686" s="1"/>
       <c r="B686" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="687" customHeight="1" ht="15.75">
-      <c r="A687" s="6"/>
+      <c r="A687" s="1"/>
       <c r="B687" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="688" customHeight="1" ht="15.75">
-      <c r="A688" s="6"/>
+      <c r="A688" s="1"/>
       <c r="B688" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="689" customHeight="1" ht="15.75">
-      <c r="A689" s="6"/>
+      <c r="A689" s="1"/>
       <c r="B689" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="690" customHeight="1" ht="15.75">
-      <c r="A690" s="6"/>
+      <c r="A690" s="1"/>
       <c r="B690" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="691" customHeight="1" ht="15.75">
-      <c r="A691" s="6"/>
+      <c r="A691" s="1"/>
       <c r="B691" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="692" customHeight="1" ht="15.75">
-      <c r="A692" s="6"/>
+      <c r="A692" s="1"/>
       <c r="B692" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="693" customHeight="1" ht="15.75">
-      <c r="A693" s="6"/>
+      <c r="A693" s="1"/>
       <c r="B693" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="694" customHeight="1" ht="15.75">
-      <c r="A694" s="6"/>
+      <c r="A694" s="1"/>
       <c r="B694" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="695" customHeight="1" ht="15.75">
-      <c r="A695" s="6"/>
+      <c r="A695" s="1"/>
       <c r="B695" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="696" customHeight="1" ht="15.75">
-      <c r="A696" s="6"/>
+      <c r="A696" s="1"/>
       <c r="B696" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="697" customHeight="1" ht="15.75">
-      <c r="A697" s="6"/>
+      <c r="A697" s="1"/>
       <c r="B697" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="698" customHeight="1" ht="15.75">
-      <c r="A698" s="6"/>
+      <c r="A698" s="1"/>
       <c r="B698" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="699" customHeight="1" ht="15.75">
-      <c r="A699" s="6"/>
+      <c r="A699" s="1"/>
       <c r="B699" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="700" customHeight="1" ht="15.75">
-      <c r="A700" s="6"/>
+      <c r="A700" s="1"/>
       <c r="B700" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="701" customHeight="1" ht="15.75">
-      <c r="A701" s="6"/>
+      <c r="A701" s="1"/>
       <c r="B701" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="702" customHeight="1" ht="15.75">
-      <c r="A702" s="6"/>
+      <c r="A702" s="1"/>
       <c r="B702" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="703" customHeight="1" ht="15.75">
-      <c r="A703" s="6"/>
+      <c r="A703" s="1"/>
       <c r="B703" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="704" customHeight="1" ht="15.75">
-      <c r="A704" s="6"/>
+      <c r="A704" s="1"/>
       <c r="B704" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="705" customHeight="1" ht="15.75">
-      <c r="A705" s="6"/>
+      <c r="A705" s="1"/>
       <c r="B705" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="706" customHeight="1" ht="15.75">
-      <c r="A706" s="6"/>
+      <c r="A706" s="1"/>
       <c r="B706" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="707" customHeight="1" ht="15.75">
-      <c r="A707" s="6"/>
+      <c r="A707" s="1"/>
       <c r="B707" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="708" customHeight="1" ht="15.75">
-      <c r="A708" s="6"/>
+      <c r="A708" s="1"/>
       <c r="B708" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="709" customHeight="1" ht="15.75">
-      <c r="A709" s="6"/>
+      <c r="A709" s="1"/>
       <c r="B709" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="710" customHeight="1" ht="15.75">
-      <c r="A710" s="6"/>
+      <c r="A710" s="1"/>
       <c r="B710" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="711" customHeight="1" ht="15.75">
-      <c r="A711" s="6"/>
+      <c r="A711" s="1"/>
       <c r="B711" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="712" customHeight="1" ht="15.75">
-      <c r="A712" s="6"/>
+      <c r="A712" s="1"/>
       <c r="B712" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="713" customHeight="1" ht="15.75">
-      <c r="A713" s="6"/>
+      <c r="A713" s="1"/>
       <c r="B713" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="714" customHeight="1" ht="15.75">
-      <c r="A714" s="6"/>
+      <c r="A714" s="1"/>
       <c r="B714" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="715" customHeight="1" ht="15.75">
-      <c r="A715" s="6"/>
+      <c r="A715" s="1"/>
       <c r="B715" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="716" customHeight="1" ht="15.75">
-      <c r="A716" s="6"/>
+      <c r="A716" s="1"/>
       <c r="B716" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="717" customHeight="1" ht="15.75">
-      <c r="A717" s="6"/>
+      <c r="A717" s="1"/>
       <c r="B717" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="718" customHeight="1" ht="15.75">
-      <c r="A718" s="6"/>
+      <c r="A718" s="1"/>
       <c r="B718" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="719" customHeight="1" ht="15.75">
-      <c r="A719" s="6"/>
+      <c r="A719" s="1"/>
       <c r="B719" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="720" customHeight="1" ht="15.75">
-      <c r="A720" s="6"/>
+      <c r="A720" s="1"/>
       <c r="B720" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="721" customHeight="1" ht="15.75">
-      <c r="A721" s="6"/>
+      <c r="A721" s="1"/>
       <c r="B721" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="722" customHeight="1" ht="15.75">
-      <c r="A722" s="6"/>
+      <c r="A722" s="1"/>
       <c r="B722" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="723" customHeight="1" ht="15.75">
-      <c r="A723" s="6"/>
+      <c r="A723" s="1"/>
       <c r="B723" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="724" customHeight="1" ht="15.75">
-      <c r="A724" s="6"/>
+      <c r="A724" s="1"/>
       <c r="B724" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="725" customHeight="1" ht="15.75">
-      <c r="A725" s="6"/>
+      <c r="A725" s="1"/>
       <c r="B725" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="726" customHeight="1" ht="15.75">
-      <c r="A726" s="6"/>
+      <c r="A726" s="1"/>
       <c r="B726" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="727" customHeight="1" ht="15.75">
-      <c r="A727" s="6"/>
+      <c r="A727" s="1"/>
       <c r="B727" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="728" customHeight="1" ht="15.75">
-      <c r="A728" s="6"/>
+      <c r="A728" s="1"/>
       <c r="B728" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="729" customHeight="1" ht="15.75">
-      <c r="A729" s="6"/>
+      <c r="A729" s="1"/>
       <c r="B729" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="730" customHeight="1" ht="15.75">
-      <c r="A730" s="6"/>
+      <c r="A730" s="1"/>
       <c r="B730" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="731" customHeight="1" ht="15.75">
-      <c r="A731" s="6"/>
+      <c r="A731" s="1"/>
       <c r="B731" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="732" customHeight="1" ht="15.75">
-      <c r="A732" s="6"/>
+      <c r="A732" s="1"/>
       <c r="B732" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="733" customHeight="1" ht="15.75">
-      <c r="A733" s="6"/>
+      <c r="A733" s="1"/>
       <c r="B733" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="734" customHeight="1" ht="15.75">
-      <c r="A734" s="6"/>
+      <c r="A734" s="1"/>
       <c r="B734" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="735" customHeight="1" ht="15.75">
-      <c r="A735" s="6"/>
+      <c r="A735" s="1"/>
       <c r="B735" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="736" customHeight="1" ht="15.75">
-      <c r="A736" s="6"/>
+      <c r="A736" s="1"/>
       <c r="B736" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="737" customHeight="1" ht="15.75">
-      <c r="A737" s="6"/>
+      <c r="A737" s="1"/>
       <c r="B737" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="738" customHeight="1" ht="15.75">
-      <c r="A738" s="6"/>
+      <c r="A738" s="1"/>
       <c r="B738" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="739" customHeight="1" ht="15.75">
-      <c r="A739" s="6"/>
+      <c r="A739" s="1"/>
       <c r="B739" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="740" customHeight="1" ht="15.75">
-      <c r="A740" s="6"/>
+      <c r="A740" s="1"/>
       <c r="B740" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="741" customHeight="1" ht="15.75">
-      <c r="A741" s="6"/>
+      <c r="A741" s="1"/>
       <c r="B741" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="742" customHeight="1" ht="15.75">
-      <c r="A742" s="6"/>
+      <c r="A742" s="1"/>
       <c r="B742" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="743" customHeight="1" ht="15.75">
-      <c r="A743" s="6"/>
+      <c r="A743" s="1"/>
       <c r="B743" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="744" customHeight="1" ht="15.75">
-      <c r="A744" s="6"/>
+      <c r="A744" s="1"/>
       <c r="B744" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="745" customHeight="1" ht="15.75">
-      <c r="A745" s="6"/>
+      <c r="A745" s="1"/>
       <c r="B745" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="746" customHeight="1" ht="15.75">
-      <c r="A746" s="6"/>
+      <c r="A746" s="1"/>
       <c r="B746" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="747" customHeight="1" ht="15.75">
-      <c r="A747" s="6"/>
+      <c r="A747" s="1"/>
       <c r="B747" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="748" customHeight="1" ht="15.75">
-      <c r="A748" s="6"/>
+      <c r="A748" s="1"/>
       <c r="B748" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="749" customHeight="1" ht="15.75">
-      <c r="A749" s="6"/>
+      <c r="A749" s="1"/>
       <c r="B749" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="750" customHeight="1" ht="15.75">
-      <c r="A750" s="6"/>
+      <c r="A750" s="1"/>
       <c r="B750" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="751" customHeight="1" ht="15.75">
-      <c r="A751" s="6"/>
+      <c r="A751" s="1"/>
       <c r="B751" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="752" customHeight="1" ht="15.75">
-      <c r="A752" s="6"/>
+      <c r="A752" s="1"/>
       <c r="B752" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="753" customHeight="1" ht="15.75">
-      <c r="A753" s="6"/>
+      <c r="A753" s="1"/>
       <c r="B753" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="754" customHeight="1" ht="15.75">
-      <c r="A754" s="6"/>
+      <c r="A754" s="1"/>
       <c r="B754" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="755" customHeight="1" ht="15.75">
-      <c r="A755" s="6"/>
+      <c r="A755" s="1"/>
       <c r="B755" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="756" customHeight="1" ht="15.75">
-      <c r="A756" s="6"/>
+      <c r="A756" s="1"/>
       <c r="B756" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="757" customHeight="1" ht="15.75">
-      <c r="A757" s="6"/>
+      <c r="A757" s="1"/>
       <c r="B757" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="758" customHeight="1" ht="15.75">
-      <c r="A758" s="6"/>
+      <c r="A758" s="1"/>
       <c r="B758" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="759" customHeight="1" ht="15.75">
-      <c r="A759" s="6"/>
+      <c r="A759" s="1"/>
       <c r="B759" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="760" customHeight="1" ht="15.75">
-      <c r="A760" s="6"/>
+      <c r="A760" s="1"/>
       <c r="B760" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="761" customHeight="1" ht="15.75">
-      <c r="A761" s="6"/>
+      <c r="A761" s="1"/>
       <c r="B761" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="762" customHeight="1" ht="15.75">
-      <c r="A762" s="6"/>
+      <c r="A762" s="1"/>
       <c r="B762" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="763" customHeight="1" ht="15.75">
-      <c r="A763" s="6"/>
+      <c r="A763" s="1"/>
       <c r="B763" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="764" customHeight="1" ht="15.75">
-      <c r="A764" s="6"/>
+      <c r="A764" s="1"/>
       <c r="B764" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="765" customHeight="1" ht="15.75">
-      <c r="A765" s="6"/>
+      <c r="A765" s="1"/>
       <c r="B765" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="766" customHeight="1" ht="15.75">
-      <c r="A766" s="6"/>
+      <c r="A766" s="1"/>
       <c r="B766" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="767" customHeight="1" ht="15.75">
-      <c r="A767" s="6"/>
+      <c r="A767" s="1"/>
       <c r="B767" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="768" customHeight="1" ht="15.75">
-      <c r="A768" s="6"/>
+      <c r="A768" s="1"/>
       <c r="B768" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="769" customHeight="1" ht="15.75">
-      <c r="A769" s="6"/>
+      <c r="A769" s="1"/>
       <c r="B769" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="770" customHeight="1" ht="15.75">
-      <c r="A770" s="6"/>
+      <c r="A770" s="1"/>
       <c r="B770" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="771" customHeight="1" ht="15.75">
-      <c r="A771" s="6"/>
+      <c r="A771" s="1"/>
       <c r="B771" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="772" customHeight="1" ht="15.75">
-      <c r="A772" s="6"/>
+      <c r="A772" s="1"/>
       <c r="B772" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="773" customHeight="1" ht="15.75">
-      <c r="A773" s="6"/>
+      <c r="A773" s="1"/>
       <c r="B773" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="774" customHeight="1" ht="15.75">
-      <c r="A774" s="6"/>
+      <c r="A774" s="1"/>
       <c r="B774" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="775" customHeight="1" ht="15.75">
-      <c r="A775" s="6"/>
+      <c r="A775" s="1"/>
       <c r="B775" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="776" customHeight="1" ht="15.75">
-      <c r="A776" s="6"/>
+      <c r="A776" s="1"/>
       <c r="B776" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="777" customHeight="1" ht="15.75">
-      <c r="A777" s="6"/>
+      <c r="A777" s="1"/>
       <c r="B777" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="778" customHeight="1" ht="15.75">
-      <c r="A778" s="6"/>
+      <c r="A778" s="1"/>
       <c r="B778" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="779" customHeight="1" ht="15.75">
-      <c r="A779" s="6"/>
+      <c r="A779" s="1"/>
       <c r="B779" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="780" customHeight="1" ht="15.75">
-      <c r="A780" s="6"/>
+      <c r="A780" s="1"/>
       <c r="B780" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="781" customHeight="1" ht="15.75">
-      <c r="A781" s="6"/>
+      <c r="A781" s="1"/>
       <c r="B781" s="2"/>
     </row>
   </sheetData>
@@ -3579,11 +3540,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -3591,59 +3552,59 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
     </row>
@@ -4861,87 +4822,59 @@
     </row>
     <row x14ac:dyDescent="0.25" r="319" customHeight="1" ht="18.75">
       <c r="A319" s="1"/>
-      <c r="B319" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B319" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="320" customHeight="1" ht="18.75">
       <c r="A320" s="1"/>
-      <c r="B320" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B320" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="321" customHeight="1" ht="18.75">
       <c r="A321" s="1"/>
-      <c r="B321" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B321" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="322" customHeight="1" ht="18.75">
       <c r="A322" s="1"/>
-      <c r="B322" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B322" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="323" customHeight="1" ht="18.75">
       <c r="A323" s="1"/>
-      <c r="B323" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B323" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="324" customHeight="1" ht="18.75">
       <c r="A324" s="1"/>
-      <c r="B324" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B324" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="325" customHeight="1" ht="18.75">
       <c r="A325" s="1"/>
-      <c r="B325" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B325" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="326" customHeight="1" ht="18.75">
       <c r="A326" s="1"/>
-      <c r="B326" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B326" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="327" customHeight="1" ht="18.75">
       <c r="A327" s="1"/>
-      <c r="B327" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B327" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="328" customHeight="1" ht="18.75">
       <c r="A328" s="1"/>
-      <c r="B328" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B328" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="329" customHeight="1" ht="18.75">
       <c r="A329" s="1"/>
-      <c r="B329" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B329" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="330" customHeight="1" ht="18.75">
       <c r="A330" s="1"/>
-      <c r="B330" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B330" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="331" customHeight="1" ht="18.75">
       <c r="A331" s="1"/>
-      <c r="B331" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B331" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="332" customHeight="1" ht="18.75">
       <c r="A332" s="1"/>
-      <c r="B332" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B332" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>